<commit_message>
Fixing default problem 4 (in default directory). Still not working. Ready to work on github issue #36.
</commit_message>
<xml_diff>
--- a/default/4_sut_multi_year_rcot_cap_new/input_data/input_data.xlsx
+++ b/default/4_sut_multi_year_rcot_cap_new/input_data/input_data.xlsx
@@ -5,24 +5,24 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\default\3_sut_multi_year_rcot_cap\input_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\default\4_sut_multi_year_rcot_cap_new\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A533B7-458E-4081-A9A1-89FC95F9DB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AC95C7-439C-43A3-99B5-3FDF62C7609F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="d" sheetId="1" r:id="rId1"/>
     <sheet name="u" sheetId="2" r:id="rId2"/>
     <sheet name="c" sheetId="3" r:id="rId3"/>
-    <sheet name="c_start" sheetId="4" r:id="rId4"/>
-    <sheet name="lf_range" sheetId="5" r:id="rId5"/>
-    <sheet name="Y" sheetId="6" r:id="rId6"/>
-    <sheet name="e" sheetId="7" r:id="rId7"/>
+    <sheet name="Y" sheetId="4" r:id="rId4"/>
+    <sheet name="c_start" sheetId="5" r:id="rId5"/>
+    <sheet name="e" sheetId="6" r:id="rId6"/>
+    <sheet name="lf_range" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Y!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Y!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -82,6 +82,36 @@
     <t>Operational costs</t>
   </si>
   <si>
+    <t>y_Name</t>
+  </si>
+  <si>
+    <t>td_Name</t>
+  </si>
+  <si>
+    <t>y1</t>
+  </si>
+  <si>
+    <t>households</t>
+  </si>
+  <si>
+    <t>y2</t>
+  </si>
+  <si>
+    <t>y3</t>
+  </si>
+  <si>
+    <t>y4</t>
+  </si>
+  <si>
+    <t>y5</t>
+  </si>
+  <si>
+    <t>e_Name</t>
+  </si>
+  <si>
+    <t>CO2 emissions</t>
+  </si>
+  <si>
     <t>lf_Name</t>
   </si>
   <si>
@@ -89,36 +119,6 @@
   </si>
   <si>
     <t>lf min</t>
-  </si>
-  <si>
-    <t>y_Name</t>
-  </si>
-  <si>
-    <t>td_Name</t>
-  </si>
-  <si>
-    <t>y1</t>
-  </si>
-  <si>
-    <t>households</t>
-  </si>
-  <si>
-    <t>y2</t>
-  </si>
-  <si>
-    <t>y3</t>
-  </si>
-  <si>
-    <t>y4</t>
-  </si>
-  <si>
-    <t>y5</t>
-  </si>
-  <si>
-    <t>e_Name</t>
-  </si>
-  <si>
-    <t>CO2 emissions</t>
   </si>
 </sst>
 </file>
@@ -489,13 +489,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="2.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.08984375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -677,17 +670,10 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E7"/>
+      <selection activeCell="E2" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="2.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.08984375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -818,17 +804,10 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E2" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="2.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.08984375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -956,10 +935,253 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="15.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="2">
+        <v>508022.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="2">
+        <v>518182.64399999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="2">
+        <v>528546.29688000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="2">
+        <v>539117.22281760001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="2">
+        <v>549899.56727395195</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0300-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F11">
+      <sortCondition ref="D1"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1017,143 +1239,6 @@
         <v>11</v>
       </c>
       <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="4" max="4" width="21.6328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7">
         <v>0</v>
       </c>
     </row>
@@ -1164,22 +1249,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="E2" sqref="E2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="2.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1187,216 +1265,64 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4">
         <v>20</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="2">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="2">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="2">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="2">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="2">
-        <v>508022.2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="2">
-        <v>518182.64399999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="2">
-        <v>528546.29688000004</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="2">
-        <v>539117.22281760001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="2">
-        <v>549899.56727395195</v>
       </c>
     </row>
   </sheetData>
@@ -1406,10 +1332,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+      <selection activeCell="E2" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1422,10 +1348,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -1439,13 +1365,13 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="E2">
-        <v>50</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1456,13 +1382,13 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1473,13 +1399,64 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
         <v>29</v>
       </c>
-      <c r="E4">
-        <v>20</v>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>